<commit_message>
adding status (bday or anniversary)
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Birthday_Wisher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA35D05-87D2-4990-B6D7-1D3C7A481F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456E6AC9-7D4F-4BC2-9DED-A5D811F18FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Sno</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -40,6 +37,15 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>Marriage Anniversary</t>
+  </si>
+  <si>
     <t>ABC</t>
   </si>
   <si>
@@ -47,6 +53,15 @@
   </si>
   <si>
     <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>Happy marriage anniversary dear XYZ :)</t>
+  </si>
+  <si>
+    <t>xyz@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -56,7 +71,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +83,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -86,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -109,18 +130,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -427,15 +462,12 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -454,95 +486,114 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>37081</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>2020</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>37081</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>37082</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>2020</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
-        <v>2020</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="2"/>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="2"/>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="2"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="2"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="2"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="2"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="2"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="2"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="2"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="2"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C22" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{34DF117D-FD5D-4FE4-9C37-3688F4D8A5EC}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1164C001-423F-4EDB-87C5-1E7267333C81}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{0DA033F7-8935-4554-B338-07D337A958F6}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
whatsapp msg sender updated, now send using pywhatkit module
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Birthday_Wisher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456E6AC9-7D4F-4BC2-9DED-A5D811F18FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B255042-2DBC-47C0-B465-6D19BF1FD6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -40,28 +40,31 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Happy birthday dear ABC :)</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Marriage Anniversary</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>Happy marriage anniversary dear XYZ :)</t>
+  </si>
+  <si>
+    <t>xyz@gmail.com</t>
+  </si>
+  <si>
     <t>Birthday</t>
-  </si>
-  <si>
-    <t>Marriage Anniversary</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>Happy birthday dear ABC :)</t>
-  </si>
-  <si>
-    <t>abc@gmail.com</t>
-  </si>
-  <si>
-    <t>XYZ</t>
-  </si>
-  <si>
-    <t>Happy marriage anniversary dear XYZ :)</t>
-  </si>
-  <si>
-    <t>xyz@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -69,9 +72,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,20 +87,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -107,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,35 +119,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -459,15 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -486,29 +458,34 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>37081</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>2020</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>1234567890</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -524,76 +501,17 @@
       <c r="D3">
         <v>2020</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>9876543210</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{1164C001-423F-4EDB-87C5-1E7267333C81}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{0DA033F7-8935-4554-B338-07D337A958F6}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>